<commit_message>
Fehler behoben, IG läuft
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-t-cabs-device-beatmungsgeraet.xlsx
+++ b/output/StructureDefinition-t-cabs-device-beatmungsgeraet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="379">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-25T16:42:03+01:00</t>
+    <t>2025-04-02T15:35:32+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -254,7 +254,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Device.id</t>
@@ -298,10 +298,6 @@
     <t>Resource.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
@@ -419,6 +415,67 @@
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
   </si>
   <si>
+    <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>Device.modifierExtension</t>
+  </si>
+  <si>
+    <t>Extensions that cannot be ignored</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+  </si>
+  <si>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
+  </si>
+  <si>
+    <t>DomainResource.modifierExtension</t>
+  </si>
+  <si>
+    <t>Device.identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier
+</t>
+  </si>
+  <si>
+    <t>Instance identifier</t>
+  </si>
+  <si>
+    <t>Alternativer Identifier zur Seriennummer</t>
+  </si>
+  <si>
+    <t>The barcode string from a barcode present on a device label or package may identify the instance, include names given to the device in local usage, or may identify the type of device. If the identifier identifies the type of device, Device.type element should be used.</t>
+  </si>
+  <si>
+    <t>Device.identifier.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>Device.identifier.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
     <t xml:space="preserve">value:url}
 </t>
   </si>
@@ -427,67 +484,6 @@
   </si>
   <si>
     <t>open</t>
-  </si>
-  <si>
-    <t>DomainResource.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Device.modifierExtension</t>
-  </si>
-  <si>
-    <t>Extensions that cannot be ignored</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
-Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
-  </si>
-  <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
-  </si>
-  <si>
-    <t>DomainResource.modifierExtension</t>
-  </si>
-  <si>
-    <t>Device.identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier
-</t>
-  </si>
-  <si>
-    <t>Instance identifier</t>
-  </si>
-  <si>
-    <t>Alternativer Identifier zur Seriennummer</t>
-  </si>
-  <si>
-    <t>The barcode string from a barcode present on a device label or package may identify the instance, include names given to the device in local usage, or may identify the type of device. If the identifier identifies the type of device, Device.type element should be used.</t>
-  </si>
-  <si>
-    <t>Device.identifier.id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>Device.identifier.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>Element.extension</t>
@@ -610,15 +606,7 @@
     <t>Time period during which identifier is/was valid for use.</t>
   </si>
   <si>
-    <t>A Period specifies a range of time; the context of use will specify whether the entire range applies (e.g. "the patient was an inpatient of the hospital for this time range") or one value from the range applies (e.g. "give to the patient between these two times").
-Period is not used for a duration (a measure of elapsed time). See [Duration](http://hl7.org/fhir/R4/datatypes.html#Duration).</t>
-  </si>
-  <si>
     <t>Identifier.period</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-per-1:If present, start SHALL have a lower value than end {start.hasValue().not() or end.hasValue().not() or (start &lt;= end)}</t>
   </si>
   <si>
     <t>Device.identifier.assigner</t>
@@ -640,10 +628,6 @@
     <t>Identifier.assigner</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ref-1:SHALL have a contained resource if a local reference is provided {reference.startsWith('#').not() or (reference.substring(1).trace('url') in %rootResource.contained.id.trace('ids'))}</t>
-  </si>
-  <si>
     <t>Device.definition</t>
   </si>
   <si>
@@ -657,9 +641,6 @@
     <t>The reference to the definition for the device.</t>
   </si>
   <si>
-    <t>References SHALL be a reference to an actual FHIR resource, and SHALL be resolveable (allowing for access control, temporary unavailability, etc.). Resolution can be either by retrieval from the URL, or, where applicable by resource type, by treating an absolute reference as a canonical URL and looking it up in a local registry/repository.</t>
-  </si>
-  <si>
     <t>Device.udiCarrier</t>
   </si>
   <si>
@@ -710,9 +691,6 @@
   </si>
   <si>
     <t>The device identifier (DI) is a mandatory, fixed portion of a UDI that identifies the labeler and the specific version or model of a device.</t>
-  </si>
-  <si>
-    <t>Note that FHIR strings SHALL NOT exceed 1MB in size</t>
   </si>
   <si>
     <t>Device.udiCarrier.issuer</t>
@@ -736,9 +714,6 @@
 http://hl7.org/fhir/NamingSystem/iccbba-other-di.</t>
   </si>
   <si>
-    <t>see http://en.wikipedia.org/wiki/Uniform_resource_identifier</t>
-  </si>
-  <si>
     <t>Device.udiCarrier.jurisdiction</t>
   </si>
   <si>
@@ -830,9 +805,6 @@
   </si>
   <si>
     <t>Reason for the dtatus of the Device availability.</t>
-  </si>
-  <si>
-    <t>Not all terminology uses fit this general pattern. In some cases, models should not use CodeableConcept and use Coding directly and provide their own structure for managing text, codings, translations and the relationship between elements and pre- and post-coordination.</t>
   </si>
   <si>
     <t>The availability status reason of the device.</t>
@@ -1143,13 +1115,6 @@
     <t>Property value as a quantity.</t>
   </si>
   <si>
-    <t>The context of use may frequently define what kind of quantity this is and therefore what kind of units can be used. The context of use may also restrict the values for the comparator.</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-qty-3:If a code for the unit is present, the system SHALL also be present {code.empty() or system.exists()}</t>
-  </si>
-  <si>
     <t>Device.property.valueCode</t>
   </si>
   <si>
@@ -1210,10 +1175,6 @@
     <t>used for troubleshooting etc.</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-cpt-2:A system is required if a value is provided. {value.empty() or system.exists()}</t>
-  </si>
-  <si>
     <t>Device.location</t>
   </si>
   <si>
@@ -1253,9 +1214,6 @@
   </si>
   <si>
     <t>Descriptive information, usage information or implantation information that is not captured in an existing element.</t>
-  </si>
-  <si>
-    <t>For systems that do not have structured annotations, they can simply communicate a single annotation with no author or time.  This element may need to be included in narrative because of the potential for modifying information.  *Annotations SHOULD NOT* be used to communicate "modifying" information that could be computable. (This is a SHOULD because enforcing user behavior is nearly impossible).</t>
   </si>
   <si>
     <t>Device.safety</t>
@@ -2049,18 +2007,18 @@
         <v>80</v>
       </c>
       <c r="AI4" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ4" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ4" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -2083,16 +2041,16 @@
         <v>81</v>
       </c>
       <c r="K5" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="L5" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="L5" t="s" s="2">
+      <c r="M5" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="M5" t="s" s="2">
+      <c r="N5" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="N5" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
@@ -2142,7 +2100,7 @@
         <v>20</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>73</v>
@@ -2151,18 +2109,18 @@
         <v>80</v>
       </c>
       <c r="AI5" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ5" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ5" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -2185,16 +2143,16 @@
         <v>20</v>
       </c>
       <c r="K6" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="L6" t="s" s="2">
         <v>101</v>
       </c>
-      <c r="L6" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="M6" t="s" s="2">
+      <c r="N6" t="s" s="2">
         <v>103</v>
-      </c>
-      <c r="N6" t="s" s="2">
-        <v>104</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -2220,32 +2178,32 @@
         <v>20</v>
       </c>
       <c r="X6" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="Y6" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="Y6" t="s" s="2">
+      <c r="Z6" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="Z6" t="s" s="2">
+      <c r="AA6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF6" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="AA6" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB6" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC6" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF6" t="s" s="2">
-        <v>108</v>
-      </c>
       <c r="AG6" t="s" s="2">
         <v>73</v>
       </c>
@@ -2253,22 +2211,22 @@
         <v>80</v>
       </c>
       <c r="AI6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ6" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ6" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
@@ -2287,16 +2245,16 @@
         <v>20</v>
       </c>
       <c r="K7" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="L7" t="s" s="2">
         <v>111</v>
       </c>
-      <c r="L7" t="s" s="2">
+      <c r="M7" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="M7" t="s" s="2">
+      <c r="N7" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="N7" t="s" s="2">
-        <v>114</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -2346,7 +2304,7 @@
         <v>20</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>73</v>
@@ -2355,22 +2313,22 @@
         <v>80</v>
       </c>
       <c r="AI7" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
@@ -2389,16 +2347,16 @@
         <v>20</v>
       </c>
       <c r="K8" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="L8" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="L8" t="s" s="2">
+      <c r="M8" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="M8" t="s" s="2">
+      <c r="N8" t="s" s="2">
         <v>120</v>
-      </c>
-      <c r="N8" t="s" s="2">
-        <v>121</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -2448,7 +2406,7 @@
         <v>20</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>73</v>
@@ -2465,14 +2423,14 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
@@ -2491,16 +2449,16 @@
         <v>20</v>
       </c>
       <c r="K9" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L9" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="M9" t="s" s="2">
         <v>126</v>
       </c>
-      <c r="M9" t="s" s="2">
+      <c r="N9" t="s" s="2">
         <v>127</v>
-      </c>
-      <c r="N9" t="s" s="2">
-        <v>128</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
@@ -2538,19 +2496,19 @@
         <v>20</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="AD9" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>73</v>
@@ -2559,22 +2517,22 @@
         <v>74</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
@@ -2593,19 +2551,19 @@
         <v>20</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O10" t="s" s="2">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P10" t="s" s="2">
         <v>20</v>
@@ -2642,19 +2600,19 @@
         <v>20</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="AD10" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>73</v>
@@ -2663,18 +2621,18 @@
         <v>74</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2697,16 +2655,16 @@
         <v>20</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" t="s" s="2">
@@ -2756,7 +2714,7 @@
         <v>20</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>73</v>
@@ -2765,18 +2723,18 @@
         <v>74</v>
       </c>
       <c r="AI11" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ11" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ11" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2799,13 +2757,13 @@
         <v>20</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -2856,7 +2814,7 @@
         <v>20</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>73</v>
@@ -2873,14 +2831,14 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
@@ -2899,16 +2857,16 @@
         <v>20</v>
       </c>
       <c r="K13" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L13" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="L13" t="s" s="2">
-        <v>126</v>
-      </c>
       <c r="M13" t="s" s="2">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
@@ -2946,19 +2904,19 @@
         <v>20</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="AC13" t="s" s="2">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="AD13" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>73</v>
@@ -2967,18 +2925,18 @@
         <v>74</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3001,19 +2959,19 @@
         <v>81</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L14" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="M14" t="s" s="2">
         <v>153</v>
       </c>
-      <c r="M14" t="s" s="2">
+      <c r="N14" t="s" s="2">
         <v>154</v>
       </c>
-      <c r="N14" t="s" s="2">
+      <c r="O14" t="s" s="2">
         <v>155</v>
-      </c>
-      <c r="O14" t="s" s="2">
-        <v>156</v>
       </c>
       <c r="P14" t="s" s="2">
         <v>20</v>
@@ -3038,32 +2996,32 @@
         <v>20</v>
       </c>
       <c r="X14" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="Y14" t="s" s="2">
         <v>157</v>
       </c>
-      <c r="Y14" t="s" s="2">
+      <c r="Z14" t="s" s="2">
         <v>158</v>
       </c>
-      <c r="Z14" t="s" s="2">
+      <c r="AA14" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB14" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC14" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD14" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE14" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF14" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="AA14" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB14" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC14" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD14" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE14" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF14" t="s" s="2">
-        <v>160</v>
-      </c>
       <c r="AG14" t="s" s="2">
         <v>73</v>
       </c>
@@ -3071,18 +3029,18 @@
         <v>80</v>
       </c>
       <c r="AI14" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ14" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3105,19 +3063,19 @@
         <v>81</v>
       </c>
       <c r="K15" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="L15" t="s" s="2">
         <v>162</v>
       </c>
-      <c r="L15" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="M15" t="s" s="2">
+      <c r="N15" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="N15" t="s" s="2">
+      <c r="O15" t="s" s="2">
         <v>165</v>
-      </c>
-      <c r="O15" t="s" s="2">
-        <v>166</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>20</v>
@@ -3127,47 +3085,47 @@
         <v>20</v>
       </c>
       <c r="S15" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="T15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X15" t="s" s="2">
         <v>167</v>
       </c>
-      <c r="T15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X15" t="s" s="2">
+      <c r="Y15" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="Y15" t="s" s="2">
+      <c r="Z15" t="s" s="2">
         <v>169</v>
       </c>
-      <c r="Z15" t="s" s="2">
+      <c r="AA15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF15" t="s" s="2">
         <v>170</v>
       </c>
-      <c r="AA15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF15" t="s" s="2">
-        <v>171</v>
-      </c>
       <c r="AG15" t="s" s="2">
         <v>73</v>
       </c>
@@ -3175,18 +3133,18 @@
         <v>80</v>
       </c>
       <c r="AI15" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ15" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ15" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3209,19 +3167,19 @@
         <v>81</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L16" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="M16" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="M16" t="s" s="2">
+      <c r="N16" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="N16" t="s" s="2">
+      <c r="O16" t="s" s="2">
         <v>175</v>
-      </c>
-      <c r="O16" t="s" s="2">
-        <v>176</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>20</v>
@@ -3234,44 +3192,44 @@
         <v>20</v>
       </c>
       <c r="T16" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="U16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF16" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="U16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE16" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF16" t="s" s="2">
-        <v>178</v>
-      </c>
       <c r="AG16" t="s" s="2">
         <v>73</v>
       </c>
@@ -3279,18 +3237,18 @@
         <v>80</v>
       </c>
       <c r="AI16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ16" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3313,16 +3271,16 @@
         <v>81</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L17" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="M17" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>181</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>182</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" t="s" s="2">
@@ -3336,44 +3294,44 @@
         <v>20</v>
       </c>
       <c r="T17" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="U17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF17" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="U17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE17" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF17" t="s" s="2">
-        <v>184</v>
-      </c>
       <c r="AG17" t="s" s="2">
         <v>73</v>
       </c>
@@ -3381,18 +3339,18 @@
         <v>80</v>
       </c>
       <c r="AI17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ17" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3415,17 +3373,15 @@
         <v>81</v>
       </c>
       <c r="K18" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="L18" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="L18" t="s" s="2">
+      <c r="M18" t="s" s="2">
         <v>187</v>
       </c>
-      <c r="M18" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="N18" t="s" s="2">
-        <v>189</v>
-      </c>
+      <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
         <v>20</v>
@@ -3474,7 +3430,7 @@
         <v>20</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>73</v>
@@ -3483,18 +3439,18 @@
         <v>80</v>
       </c>
       <c r="AI18" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ18" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ18" t="s" s="2">
-        <v>191</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3517,16 +3473,16 @@
         <v>81</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="M19" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="N19" t="s" s="2">
         <v>193</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>196</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
@@ -3576,7 +3532,7 @@
         <v>20</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>73</v>
@@ -3585,18 +3541,18 @@
         <v>80</v>
       </c>
       <c r="AI19" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ19" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ19" t="s" s="2">
-        <v>198</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3619,17 +3575,15 @@
         <v>20</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
         <v>20</v>
@@ -3678,7 +3632,7 @@
         <v>20</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>73</v>
@@ -3687,18 +3641,18 @@
         <v>80</v>
       </c>
       <c r="AI20" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ20" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ20" t="s" s="2">
-        <v>198</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3721,16 +3675,16 @@
         <v>81</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -3780,7 +3734,7 @@
         <v>20</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>73</v>
@@ -3789,18 +3743,18 @@
         <v>74</v>
       </c>
       <c r="AI21" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3823,13 +3777,13 @@
         <v>20</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -3880,7 +3834,7 @@
         <v>20</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>73</v>
@@ -3897,14 +3851,14 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
@@ -3923,16 +3877,16 @@
         <v>20</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="L23" t="s" s="2">
-        <v>126</v>
-      </c>
       <c r="M23" t="s" s="2">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -3970,19 +3924,19 @@
         <v>20</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="AC23" t="s" s="2">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="AD23" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>73</v>
@@ -3991,22 +3945,22 @@
         <v>74</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4025,19 +3979,19 @@
         <v>81</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>20</v>
@@ -4086,7 +4040,7 @@
         <v>20</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>73</v>
@@ -4095,22 +4049,22 @@
         <v>74</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4129,17 +4083,15 @@
         <v>81</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
         <v>20</v>
@@ -4188,7 +4140,7 @@
         <v>20</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>73</v>
@@ -4197,22 +4149,22 @@
         <v>80</v>
       </c>
       <c r="AI25" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ25" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ25" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
@@ -4231,17 +4183,15 @@
         <v>20</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>225</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
         <v>20</v>
@@ -4290,7 +4240,7 @@
         <v>20</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>73</v>
@@ -4299,18 +4249,18 @@
         <v>80</v>
       </c>
       <c r="AI26" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ26" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ26" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4333,19 +4283,17 @@
         <v>20</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>225</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>20</v>
@@ -4394,7 +4342,7 @@
         <v>20</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>73</v>
@@ -4403,22 +4351,22 @@
         <v>80</v>
       </c>
       <c r="AI27" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ27" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ27" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
@@ -4437,16 +4385,16 @@
         <v>81</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4496,7 +4444,7 @@
         <v>20</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>73</v>
@@ -4505,22 +4453,22 @@
         <v>80</v>
       </c>
       <c r="AI28" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ28" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
@@ -4539,16 +4487,16 @@
         <v>81</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -4598,7 +4546,7 @@
         <v>20</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>73</v>
@@ -4607,18 +4555,18 @@
         <v>80</v>
       </c>
       <c r="AI29" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4641,19 +4589,17 @@
         <v>20</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="P30" t="s" s="2">
         <v>20</v>
@@ -4678,13 +4624,13 @@
         <v>20</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="Z30" t="s" s="2">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>20</v>
@@ -4702,7 +4648,7 @@
         <v>20</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>73</v>
@@ -4711,18 +4657,18 @@
         <v>80</v>
       </c>
       <c r="AI30" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ30" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -4745,16 +4691,16 @@
         <v>81</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -4780,13 +4726,13 @@
         <v>20</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="Z31" t="s" s="2">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>20</v>
@@ -4804,7 +4750,7 @@
         <v>20</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>73</v>
@@ -4813,18 +4759,18 @@
         <v>80</v>
       </c>
       <c r="AI31" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -4847,17 +4793,15 @@
         <v>20</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>256</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
         <v>20</v>
@@ -4882,13 +4826,13 @@
         <v>20</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="Z32" t="s" s="2">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="AA32" t="s" s="2">
         <v>20</v>
@@ -4906,7 +4850,7 @@
         <v>20</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>73</v>
@@ -4915,22 +4859,22 @@
         <v>74</v>
       </c>
       <c r="AI32" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
@@ -4949,16 +4893,16 @@
         <v>20</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -5008,7 +4952,7 @@
         <v>20</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>73</v>
@@ -5017,18 +4961,18 @@
         <v>80</v>
       </c>
       <c r="AI33" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ33" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ33" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5051,17 +4995,15 @@
         <v>20</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
         <v>20</v>
@@ -5110,7 +5052,7 @@
         <v>20</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>73</v>
@@ -5119,18 +5061,18 @@
         <v>80</v>
       </c>
       <c r="AI34" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ34" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5153,13 +5095,13 @@
         <v>20</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -5210,7 +5152,7 @@
         <v>20</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>73</v>
@@ -5219,18 +5161,18 @@
         <v>80</v>
       </c>
       <c r="AI35" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5253,13 +5195,13 @@
         <v>20</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -5310,7 +5252,7 @@
         <v>20</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>73</v>
@@ -5319,18 +5261,18 @@
         <v>80</v>
       </c>
       <c r="AI36" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5353,17 +5295,15 @@
         <v>20</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
         <v>20</v>
@@ -5412,7 +5352,7 @@
         <v>20</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>73</v>
@@ -5421,18 +5361,18 @@
         <v>80</v>
       </c>
       <c r="AI37" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ37" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ37" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5455,16 +5395,16 @@
         <v>20</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
@@ -5514,7 +5454,7 @@
         <v>20</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>73</v>
@@ -5523,18 +5463,18 @@
         <v>80</v>
       </c>
       <c r="AI38" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5557,13 +5497,13 @@
         <v>20</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -5614,7 +5554,7 @@
         <v>20</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>73</v>
@@ -5623,18 +5563,18 @@
         <v>74</v>
       </c>
       <c r="AI39" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -5657,13 +5597,13 @@
         <v>20</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -5714,7 +5654,7 @@
         <v>20</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>73</v>
@@ -5731,14 +5671,14 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -5757,16 +5697,16 @@
         <v>20</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="L41" t="s" s="2">
-        <v>126</v>
-      </c>
       <c r="M41" t="s" s="2">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -5804,19 +5744,19 @@
         <v>20</v>
       </c>
       <c r="AB41" t="s" s="2">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="AC41" t="s" s="2">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="AD41" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>73</v>
@@ -5825,22 +5765,22 @@
         <v>74</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
@@ -5859,19 +5799,19 @@
         <v>81</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>20</v>
@@ -5920,7 +5860,7 @@
         <v>20</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>73</v>
@@ -5929,22 +5869,22 @@
         <v>74</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
@@ -5963,17 +5903,15 @@
         <v>20</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
         <v>20</v>
@@ -6022,7 +5960,7 @@
         <v>20</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>80</v>
@@ -6031,18 +5969,18 @@
         <v>80</v>
       </c>
       <c r="AI43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ43" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6065,17 +6003,15 @@
         <v>20</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
         <v>20</v>
@@ -6085,7 +6021,7 @@
         <v>20</v>
       </c>
       <c r="S44" t="s" s="2">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="T44" t="s" s="2">
         <v>20</v>
@@ -6100,13 +6036,13 @@
         <v>20</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="Z44" t="s" s="2">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>20</v>
@@ -6124,7 +6060,7 @@
         <v>20</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>80</v>
@@ -6133,18 +6069,18 @@
         <v>80</v>
       </c>
       <c r="AI44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ44" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6167,17 +6103,15 @@
         <v>20</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
         <v>20</v>
@@ -6226,7 +6160,7 @@
         <v>20</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>73</v>
@@ -6235,18 +6169,18 @@
         <v>80</v>
       </c>
       <c r="AI45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ45" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6269,16 +6203,16 @@
         <v>20</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -6328,7 +6262,7 @@
         <v>20</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>73</v>
@@ -6337,18 +6271,18 @@
         <v>80</v>
       </c>
       <c r="AI46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ46" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6371,17 +6305,15 @@
         <v>20</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>256</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="N47" s="2"/>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
         <v>20</v>
@@ -6391,7 +6323,7 @@
         <v>20</v>
       </c>
       <c r="S47" t="s" s="2">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="T47" t="s" s="2">
         <v>20</v>
@@ -6406,13 +6338,13 @@
         <v>20</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>20</v>
@@ -6430,7 +6362,7 @@
         <v>20</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>73</v>
@@ -6439,18 +6371,18 @@
         <v>80</v>
       </c>
       <c r="AI47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ47" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -6473,13 +6405,13 @@
         <v>20</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -6530,7 +6462,7 @@
         <v>20</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>73</v>
@@ -6539,18 +6471,18 @@
         <v>74</v>
       </c>
       <c r="AI48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ48" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -6573,13 +6505,13 @@
         <v>20</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -6630,7 +6562,7 @@
         <v>20</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>73</v>
@@ -6647,14 +6579,14 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
@@ -6673,16 +6605,16 @@
         <v>20</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="L50" t="s" s="2">
-        <v>126</v>
-      </c>
       <c r="M50" t="s" s="2">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
@@ -6720,19 +6652,19 @@
         <v>20</v>
       </c>
       <c r="AB50" t="s" s="2">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="AC50" t="s" s="2">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="AD50" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>73</v>
@@ -6741,22 +6673,22 @@
         <v>74</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s" s="2">
@@ -6775,19 +6707,19 @@
         <v>81</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O51" t="s" s="2">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>20</v>
@@ -6836,7 +6768,7 @@
         <v>20</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>73</v>
@@ -6845,22 +6777,22 @@
         <v>74</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s" s="2">
@@ -6879,17 +6811,15 @@
         <v>20</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>256</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
         <v>20</v>
@@ -6938,7 +6868,7 @@
         <v>20</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>80</v>
@@ -6947,18 +6877,18 @@
         <v>80</v>
       </c>
       <c r="AI52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -6981,17 +6911,15 @@
         <v>20</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
         <v>20</v>
@@ -7040,7 +6968,7 @@
         <v>20</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>73</v>
@@ -7049,18 +6977,18 @@
         <v>80</v>
       </c>
       <c r="AI53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -7083,13 +7011,13 @@
         <v>20</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -7140,7 +7068,7 @@
         <v>20</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>73</v>
@@ -7149,18 +7077,18 @@
         <v>74</v>
       </c>
       <c r="AI54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -7183,13 +7111,13 @@
         <v>20</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -7240,7 +7168,7 @@
         <v>20</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>73</v>
@@ -7257,14 +7185,14 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
@@ -7283,16 +7211,16 @@
         <v>20</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L56" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="L56" t="s" s="2">
-        <v>126</v>
-      </c>
       <c r="M56" t="s" s="2">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
@@ -7330,19 +7258,19 @@
         <v>20</v>
       </c>
       <c r="AB56" t="s" s="2">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="AC56" t="s" s="2">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="AD56" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>73</v>
@@ -7351,22 +7279,22 @@
         <v>74</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
@@ -7385,19 +7313,19 @@
         <v>81</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O57" t="s" s="2">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P57" t="s" s="2">
         <v>20</v>
@@ -7446,7 +7374,7 @@
         <v>20</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>73</v>
@@ -7455,22 +7383,22 @@
         <v>74</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
@@ -7489,17 +7417,15 @@
         <v>20</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>256</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="N58" s="2"/>
       <c r="O58" s="2"/>
       <c r="P58" t="s" s="2">
         <v>20</v>
@@ -7548,7 +7474,7 @@
         <v>20</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>73</v>
@@ -7557,18 +7483,18 @@
         <v>80</v>
       </c>
       <c r="AI58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ58" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ58" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -7591,13 +7517,13 @@
         <v>20</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -7648,7 +7574,7 @@
         <v>20</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>73</v>
@@ -7657,18 +7583,18 @@
         <v>80</v>
       </c>
       <c r="AI59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ59" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ59" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -7691,17 +7617,15 @@
         <v>20</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="N60" s="2"/>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
         <v>20</v>
@@ -7750,7 +7674,7 @@
         <v>20</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>80</v>
@@ -7759,18 +7683,18 @@
         <v>80</v>
       </c>
       <c r="AI60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ60" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -7793,13 +7717,13 @@
         <v>20</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -7850,7 +7774,7 @@
         <v>20</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>73</v>
@@ -7859,18 +7783,18 @@
         <v>74</v>
       </c>
       <c r="AI61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -7893,13 +7817,13 @@
         <v>20</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -7950,7 +7874,7 @@
         <v>20</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>73</v>
@@ -7967,14 +7891,14 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
@@ -7993,16 +7917,16 @@
         <v>20</v>
       </c>
       <c r="K63" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L63" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="L63" t="s" s="2">
-        <v>126</v>
-      </c>
       <c r="M63" t="s" s="2">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" t="s" s="2">
@@ -8040,19 +7964,19 @@
         <v>20</v>
       </c>
       <c r="AB63" t="s" s="2">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="AC63" t="s" s="2">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="AD63" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>73</v>
@@ -8061,22 +7985,22 @@
         <v>74</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
@@ -8095,19 +8019,19 @@
         <v>81</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O64" t="s" s="2">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P64" t="s" s="2">
         <v>20</v>
@@ -8156,7 +8080,7 @@
         <v>20</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>73</v>
@@ -8165,18 +8089,18 @@
         <v>74</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -8199,17 +8123,15 @@
         <v>20</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>256</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="N65" s="2"/>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
         <v>20</v>
@@ -8258,7 +8180,7 @@
         <v>20</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>80</v>
@@ -8267,18 +8189,18 @@
         <v>80</v>
       </c>
       <c r="AI65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ65" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ65" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -8301,17 +8223,15 @@
         <v>20</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="N66" t="s" s="2">
-        <v>350</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="N66" s="2"/>
       <c r="O66" s="2"/>
       <c r="P66" t="s" s="2">
         <v>20</v>
@@ -8360,7 +8280,7 @@
         <v>20</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>73</v>
@@ -8369,18 +8289,18 @@
         <v>74</v>
       </c>
       <c r="AI66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ66" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ66" t="s" s="2">
-        <v>351</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -8403,17 +8323,15 @@
         <v>20</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>256</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="N67" s="2"/>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
         <v>20</v>
@@ -8462,7 +8380,7 @@
         <v>20</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>73</v>
@@ -8471,18 +8389,18 @@
         <v>74</v>
       </c>
       <c r="AI67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ67" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -8505,19 +8423,17 @@
         <v>20</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="P68" t="s" s="2">
         <v>20</v>
@@ -8566,7 +8482,7 @@
         <v>20</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>73</v>
@@ -8575,18 +8491,18 @@
         <v>80</v>
       </c>
       <c r="AI68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ68" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ68" t="s" s="2">
-        <v>198</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -8609,16 +8525,16 @@
         <v>20</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" t="s" s="2">
@@ -8668,7 +8584,7 @@
         <v>20</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>73</v>
@@ -8677,18 +8593,18 @@
         <v>80</v>
       </c>
       <c r="AI69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ69" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ69" t="s" s="2">
-        <v>198</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -8711,16 +8627,16 @@
         <v>20</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
@@ -8770,7 +8686,7 @@
         <v>20</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>73</v>
@@ -8779,18 +8695,18 @@
         <v>74</v>
       </c>
       <c r="AI70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ70" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ70" t="s" s="2">
-        <v>369</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -8813,19 +8729,17 @@
         <v>20</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="P71" t="s" s="2">
         <v>20</v>
@@ -8874,7 +8788,7 @@
         <v>20</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>73</v>
@@ -8883,18 +8797,18 @@
         <v>80</v>
       </c>
       <c r="AI71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ71" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ71" t="s" s="2">
-        <v>198</v>
       </c>
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -8917,16 +8831,16 @@
         <v>20</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="N72" t="s" s="2">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="O72" s="2"/>
       <c r="P72" t="s" s="2">
@@ -8976,7 +8890,7 @@
         <v>20</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>73</v>
@@ -8985,18 +8899,18 @@
         <v>80</v>
       </c>
       <c r="AI72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ72" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ72" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -9019,17 +8933,15 @@
         <v>20</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>383</v>
-      </c>
+        <v>371</v>
+      </c>
+      <c r="N73" s="2"/>
       <c r="O73" s="2"/>
       <c r="P73" t="s" s="2">
         <v>20</v>
@@ -9078,7 +8990,7 @@
         <v>20</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>73</v>
@@ -9087,18 +8999,18 @@
         <v>74</v>
       </c>
       <c r="AI73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ73" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ73" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -9121,17 +9033,15 @@
         <v>81</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>256</v>
-      </c>
+        <v>374</v>
+      </c>
+      <c r="N74" s="2"/>
       <c r="O74" s="2"/>
       <c r="P74" t="s" s="2">
         <v>20</v>
@@ -9180,7 +9090,7 @@
         <v>20</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>73</v>
@@ -9189,18 +9099,18 @@
         <v>74</v>
       </c>
       <c r="AI74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ74" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -9223,17 +9133,15 @@
         <v>20</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="N75" s="2"/>
       <c r="O75" s="2"/>
       <c r="P75" t="s" s="2">
         <v>20</v>
@@ -9282,7 +9190,7 @@
         <v>20</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>73</v>
@@ -9291,10 +9199,10 @@
         <v>80</v>
       </c>
       <c r="AI75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ75" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="AJ75" t="s" s="2">
-        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>